<commit_message>
Transactions code transferred, ready for component support
</commit_message>
<xml_diff>
--- a/datasets/transactions.xlsx
+++ b/datasets/transactions.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M367"/>
+  <dimension ref="A1:M387"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3689,7 +3689,7 @@
           <t>Mechanics</t>
         </is>
       </c>
-      <c r="L66" t="b">
+      <c r="L66" t="n">
         <v>1</v>
       </c>
       <c r="M66" t="inlineStr">
@@ -19314,7 +19314,7 @@
         <v>44940</v>
       </c>
       <c r="C365" s="2" t="n">
-        <v>44940</v>
+        <v>44953</v>
       </c>
       <c r="D365" s="2" t="n">
         <v>44937</v>
@@ -19353,7 +19353,7 @@
       </c>
       <c r="M365" t="inlineStr">
         <is>
-          <t>Gasoline</t>
+          <t>Groceries</t>
         </is>
       </c>
     </row>
@@ -19454,6 +19454,1002 @@
           <t>nan</t>
         </is>
       </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="inlineStr">
+        <is>
+          <t>97568398-2d77-4002-8c2f-acdf0a8a247d</t>
+        </is>
+      </c>
+      <c r="B368" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C368" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D368" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="E368" s="2" t="n">
+        <v>44944</v>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>AUTOMOTIVE OUTFITTERS LL</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>Automotive</t>
+        </is>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I368" t="n">
+        <v>-125</v>
+      </c>
+      <c r="J368" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K368" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L368" t="n">
+        <v>1</v>
+      </c>
+      <c r="M368" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="inlineStr">
+        <is>
+          <t>d93ece9c-52e5-4490-ad34-3f9b4bd18f94</t>
+        </is>
+      </c>
+      <c r="B369" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C369" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D369" s="2" t="n">
+        <v>44941</v>
+      </c>
+      <c r="E369" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>76 - CF UNITED APRO LL</t>
+        </is>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I369" t="n">
+        <v>-31.43</v>
+      </c>
+      <c r="J369" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K369" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L369" t="n">
+        <v>1</v>
+      </c>
+      <c r="M369" t="inlineStr">
+        <is>
+          <t>Gasoline</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="inlineStr">
+        <is>
+          <t>84773f4c-1a95-41af-abe2-413b7c887ae5</t>
+        </is>
+      </c>
+      <c r="B370" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C370" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D370" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="E370" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>TIREBUYER.COM LLC</t>
+        </is>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>Automotive</t>
+        </is>
+      </c>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I370" t="n">
+        <v>-901.12</v>
+      </c>
+      <c r="J370" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K370" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L370" t="n">
+        <v>1</v>
+      </c>
+      <c r="M370" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="inlineStr">
+        <is>
+          <t>ea36ea7b-150c-4c90-9a91-87d5c10aeafb</t>
+        </is>
+      </c>
+      <c r="B371" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C371" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D371" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="E371" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>ALL HEART YOGA</t>
+        </is>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>Personal</t>
+        </is>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I371" t="n">
+        <v>-18</v>
+      </c>
+      <c r="J371" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K371" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L371" t="n">
+        <v>1</v>
+      </c>
+      <c r="M371" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="inlineStr">
+        <is>
+          <t>093f78da-0829-432e-a446-2d68fc919c84</t>
+        </is>
+      </c>
+      <c r="B372" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C372" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D372" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="E372" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>SP  RED LIGHT CLOTHI</t>
+        </is>
+      </c>
+      <c r="G372" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="H372" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I372" t="n">
+        <v>-99.95999999999999</v>
+      </c>
+      <c r="J372" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K372" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L372" t="n">
+        <v>1</v>
+      </c>
+      <c r="M372" t="inlineStr">
+        <is>
+          <t>Clothes</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="inlineStr">
+        <is>
+          <t>b1585b76-bdbc-42bd-870a-7a3a7b98a37f</t>
+        </is>
+      </c>
+      <c r="B373" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C373" t="inlineStr"/>
+      <c r="D373" s="2" t="n">
+        <v>44936</v>
+      </c>
+      <c r="E373" s="2" t="n">
+        <v>44937</v>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>Amazon Prime*MN5F08MU3</t>
+        </is>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>Bills &amp; Utilities</t>
+        </is>
+      </c>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I373" t="n">
+        <v>-7.49</v>
+      </c>
+      <c r="J373" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K373" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L373" t="n">
+        <v>0</v>
+      </c>
+      <c r="M373" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="inlineStr">
+        <is>
+          <t>590b148f-f7d3-418f-bce6-f587dad67736</t>
+        </is>
+      </c>
+      <c r="B374" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="C374" t="inlineStr"/>
+      <c r="D374" s="2" t="n">
+        <v>44934</v>
+      </c>
+      <c r="E374" s="2" t="n">
+        <v>44936</v>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>FASTRAK FUEL MART</t>
+        </is>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I374" t="n">
+        <v>-50.83</v>
+      </c>
+      <c r="J374" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="K374" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L374" t="n">
+        <v>0</v>
+      </c>
+      <c r="M374" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="inlineStr">
+        <is>
+          <t>3a67e11a-be27-477d-a6a3-ba56c3bf145d</t>
+        </is>
+      </c>
+      <c r="B375" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C375" t="inlineStr"/>
+      <c r="D375" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="E375" s="2" t="n">
+        <v>44944</v>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>SQ *ALOUETTE</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I375" t="n">
+        <v>-81</v>
+      </c>
+      <c r="J375" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K375" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L375" t="n">
+        <v>0</v>
+      </c>
+      <c r="M375" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="inlineStr">
+        <is>
+          <t>f150caef-916b-47ca-98c3-d2646b5266a4</t>
+        </is>
+      </c>
+      <c r="B376" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C376" t="inlineStr"/>
+      <c r="D376" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="E376" s="2" t="n">
+        <v>44944</v>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>SQ *LENTS DRAFT AND BOTTL</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I376" t="n">
+        <v>-10</v>
+      </c>
+      <c r="J376" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K376" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L376" t="n">
+        <v>0</v>
+      </c>
+      <c r="M376" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="inlineStr">
+        <is>
+          <t>58308471-6bed-44c9-8d4e-40e60625136c</t>
+        </is>
+      </c>
+      <c r="B377" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C377" t="inlineStr"/>
+      <c r="D377" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="E377" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>AUTOMATIC PAYMENT - THANK</t>
+        </is>
+      </c>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>Payment</t>
+        </is>
+      </c>
+      <c r="I377" t="n">
+        <v>947.85</v>
+      </c>
+      <c r="J377" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K377" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L377" t="n">
+        <v>0</v>
+      </c>
+      <c r="M377" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="inlineStr">
+        <is>
+          <t>78949e38-4769-4447-9d17-dcd6370f91a4</t>
+        </is>
+      </c>
+      <c r="B378" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C378" t="inlineStr"/>
+      <c r="D378" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="E378" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>TRADER JOE'S #146  QPS</t>
+        </is>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I378" t="n">
+        <v>-57.27</v>
+      </c>
+      <c r="J378" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K378" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L378" t="n">
+        <v>0</v>
+      </c>
+      <c r="M378" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="inlineStr">
+        <is>
+          <t>a4ef4656-5c8a-4fd6-ad39-227e4db6e4f7</t>
+        </is>
+      </c>
+      <c r="B379" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C379" t="inlineStr"/>
+      <c r="D379" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="E379" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>LA BUCA</t>
+        </is>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I379" t="n">
+        <v>-51</v>
+      </c>
+      <c r="J379" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K379" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L379" t="n">
+        <v>0</v>
+      </c>
+      <c r="M379" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="inlineStr">
+        <is>
+          <t>18e27e22-f487-43a4-8386-b17f9ca41b69</t>
+        </is>
+      </c>
+      <c r="B380" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C380" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D380" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="E380" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>SQ *EASTSIDE COFFEE BAR &amp;amp;</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I380" t="n">
+        <v>-10.5</v>
+      </c>
+      <c r="J380" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K380" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L380" t="n">
+        <v>1</v>
+      </c>
+      <c r="M380" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="inlineStr">
+        <is>
+          <t>73af5f61-15c1-4358-8706-3c0ee263fbf0</t>
+        </is>
+      </c>
+      <c r="B381" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C381" t="inlineStr"/>
+      <c r="D381" s="2" t="n">
+        <v>44941</v>
+      </c>
+      <c r="E381" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>SQ *SPIELMAN COFFEE ROAST</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I381" t="n">
+        <v>-4</v>
+      </c>
+      <c r="J381" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K381" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L381" t="n">
+        <v>0</v>
+      </c>
+      <c r="M381" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="inlineStr">
+        <is>
+          <t>fb4bfd21-d0f2-4366-92c7-794d28e9f225</t>
+        </is>
+      </c>
+      <c r="B382" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C382" t="inlineStr"/>
+      <c r="D382" s="2" t="n">
+        <v>44941</v>
+      </c>
+      <c r="E382" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>SQ *SPIELMAN COFFEE ROAST</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I382" t="n">
+        <v>-13.51</v>
+      </c>
+      <c r="J382" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K382" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L382" t="n">
+        <v>0</v>
+      </c>
+      <c r="M382" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="inlineStr">
+        <is>
+          <t>84ec5a1f-7e85-445e-85a3-6aa50092e3d2</t>
+        </is>
+      </c>
+      <c r="B383" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C383" t="inlineStr"/>
+      <c r="D383" s="2" t="n">
+        <v>44940</v>
+      </c>
+      <c r="E383" s="2" t="n">
+        <v>44941</v>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>SQ *BARISTA</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I383" t="n">
+        <v>-12.75</v>
+      </c>
+      <c r="J383" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K383" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L383" t="n">
+        <v>0</v>
+      </c>
+      <c r="M383" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="inlineStr">
+        <is>
+          <t>23154ca8-e412-4d2d-a2ea-e4384ca39724</t>
+        </is>
+      </c>
+      <c r="B384" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C384" t="inlineStr"/>
+      <c r="D384" s="2" t="n">
+        <v>44937</v>
+      </c>
+      <c r="E384" s="2" t="n">
+        <v>44938</v>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>TRADER JOE'S #146  QPS</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I384" t="n">
+        <v>-43.6</v>
+      </c>
+      <c r="J384" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K384" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L384" t="n">
+        <v>0</v>
+      </c>
+      <c r="M384" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="inlineStr">
+        <is>
+          <t>87ed3782-c90d-4d01-90ec-e4e2837182c2</t>
+        </is>
+      </c>
+      <c r="B385" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C385" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="D385" s="2" t="n">
+        <v>44946</v>
+      </c>
+      <c r="E385" t="inlineStr"/>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>TOYOTA MOTOR SAL PAYROLL 568349-TLS</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr"/>
+      <c r="H385" t="inlineStr"/>
+      <c r="I385" t="n">
+        <v>1926.84</v>
+      </c>
+      <c r="J385" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K385" t="inlineStr">
+        <is>
+          <t>Mechanics</t>
+        </is>
+      </c>
+      <c r="L385" t="b">
+        <v>1</v>
+      </c>
+      <c r="M385" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="inlineStr">
+        <is>
+          <t>19382a1f-7c1f-4560-bc05-e3e5ea2d94da</t>
+        </is>
+      </c>
+      <c r="B386" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C386" t="inlineStr"/>
+      <c r="D386" s="2" t="n">
+        <v>44944</v>
+      </c>
+      <c r="E386" t="inlineStr"/>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>CHASE CREDIT CRD AUTOPAY 000000000293948</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr"/>
+      <c r="H386" t="inlineStr"/>
+      <c r="I386" t="n">
+        <v>-947.85</v>
+      </c>
+      <c r="J386" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K386" t="inlineStr">
+        <is>
+          <t>Mechanics</t>
+        </is>
+      </c>
+      <c r="L386" t="n">
+        <v>0</v>
+      </c>
+      <c r="M386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="1" t="inlineStr">
+        <is>
+          <t>1a1ecf78-0135-4a27-918c-ad8929ef8c37</t>
+        </is>
+      </c>
+      <c r="B387" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="C387" t="inlineStr"/>
+      <c r="D387" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="E387" t="inlineStr"/>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>VENMO PAYMENT 1024681449816</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr"/>
+      <c r="H387" t="inlineStr"/>
+      <c r="I387" t="n">
+        <v>-29</v>
+      </c>
+      <c r="J387" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="K387" t="inlineStr">
+        <is>
+          <t>Mechanics</t>
+        </is>
+      </c>
+      <c r="L387" t="n">
+        <v>0</v>
+      </c>
+      <c r="M387" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>